<commit_message>
product list 16개씩 + security 추가
</commit_message>
<xml_diff>
--- a/구조.xlsx
+++ b/구조.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GIT\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8682A9EB-A569-4B3F-B421-0305008E5416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE92BF9F-D645-4E3D-B38C-9F7D7B46FD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="1" xr2:uid="{9DD572A8-5AF6-4191-AC26-81DE3BDAA7E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{9DD572A8-5AF6-4191-AC26-81DE3BDAA7E4}"/>
   </bookViews>
   <sheets>
     <sheet name="리액트" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>main.jsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,10 +78,6 @@
   </si>
   <si>
     <t>ModifyPage.jsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>todo폴더</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -278,6 +274,20 @@
   </si>
   <si>
     <t>MallapiApplication.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Footer.jsx
+하단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageConstants.jsx (페이징 사이즈 지정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo/products
+폴더</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -310,7 +320,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -490,13 +500,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,27 +582,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1267,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E74F87-8DD6-414F-B904-B629E1B943E5}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1283,206 +1325,224 @@
     <col min="6" max="6" width="14.75" customWidth="1"/>
     <col min="7" max="7" width="21.625" customWidth="1"/>
     <col min="8" max="8" width="31.125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="66.25" customWidth="1"/>
+    <col min="9" max="9" width="19.75" style="2" customWidth="1"/>
+    <col min="10" max="10" width="66.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+    <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="24"/>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="I3" s="25"/>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="16"/>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="25"/>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="G6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="H3:H4"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G3:G5"/>
-    <mergeCell ref="H3:H5"/>
     <mergeCell ref="E5:E12"/>
     <mergeCell ref="D5:D12"/>
     <mergeCell ref="F10:F11"/>
@@ -1493,7 +1553,6 @@
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="B3:B13"/>
-    <mergeCell ref="C3:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1505,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15A43A-C99F-42F6-8838-5B8DB14B0367}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1520,150 +1579,144 @@
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="6"/>
       <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="23"/>
+      <c r="H2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="H3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>40</v>
-      </c>
-      <c r="N3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
-        <v>49</v>
+      <c r="H4" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22" t="s">
-        <v>50</v>
+      <c r="H5" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22" t="s">
-        <v>55</v>
+      <c r="H6" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>26</v>
-      </c>
-      <c r="O6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1672,13 +1725,12 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="H7" s="16"/>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1687,8 +1739,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
@@ -1696,10 +1747,9 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="16"/>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1708,8 +1758,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="2:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
@@ -1717,22 +1766,21 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>